<commit_message>
informar cantidad de registros no insertados al cargar mal
</commit_message>
<xml_diff>
--- a/AsistManager/wwwroot/Uploads/registros.xlsx
+++ b/AsistManager/wwwroot/Uploads/registros.xlsx
@@ -38,6 +38,456 @@
   </x:si>
   <x:si>
     <x:t>Alta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reece</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shugg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>06-25331652-11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(142) 4993773</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Puku</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sí</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Selma</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gave</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10149315</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(586) 8205499</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hartebeest, coke's</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cobby</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rogeon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8956649</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-13237035-61</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(382) 6611426</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Armadillo, common long-nosed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Etti</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Boulsher</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15572339</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69-53131429-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(972) 6509150</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mongoose, banded</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vinnie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pentony</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13354602</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34-43197113-99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(295) 8322970</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ring-tailed coatimundi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maria</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Billitteri</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81217729</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26-80940595-96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(775) 2516606</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Eurasian beaver</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ashlen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>de Tocqueville</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12436626</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49-42574341-65</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(832) 8024500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Greater blue-eared starling</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alexis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Damp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>91306638</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67-34291374-92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(883) 4920125</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mockingbird, galapagos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jeromy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rielly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29177523</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20-93557794-67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(792) 9271736</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Squirrel, indian giant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reiner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37647492</x:t>
+  </x:si>
+  <x:si>
+    <x:t>76-97691202-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(703) 5961604</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Goanna lizard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stephen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Danick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>78452955</x:t>
+  </x:si>
+  <x:si>
+    <x:t>63-57238603-93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(329) 4881121</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grey fox</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hugibert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bosomworth</x:t>
+  </x:si>
+  <x:si>
+    <x:t>83756470</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64-96350335-62</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(665) 3956554</x:t>
+  </x:si>
+  <x:si>
+    <x:t>African skink</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wanids</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Du Hamel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>93963919</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50-91779460-40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(407) 1366643</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Starfish, crown of thorns</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Demetria</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wolledge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82960998</x:t>
+  </x:si>
+  <x:si>
+    <x:t>59-13274709-91</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(883) 5654742</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Square-lipped rhinoceros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Delcine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>McMillan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>66144133</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-16911837-64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(446) 2181833</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tyrant flycatcher</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shirline</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shelley</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41045523</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55-11757474-60</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(378) 8226608</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Puffin, horned</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jonas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grieger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56792120</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34-62192081-13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(533) 5560622</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Drongo, fork-tailed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Calv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gobourn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32833883</x:t>
+  </x:si>
+  <x:si>
+    <x:t>90-22862581-96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(568) 4775056</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cat, african wild</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Haleigh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Godlee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8893982</x:t>
+  </x:si>
+  <x:si>
+    <x:t>42-77773577-94</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(626) 8553839</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oriental short-clawed otter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Todd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chree</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71262655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95-14518863-58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(772) 2582295</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Starling, superb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kane</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dole</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2801641</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32-56096304-96</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(464) 2533904</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caiman, spectacled</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alvan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mingaud</x:t>
+  </x:si>
+  <x:si>
+    <x:t>89691387</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00-09784203-93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(239) 6220253</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Monster, gila</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Liam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wakeham</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33673900</x:t>
+  </x:si>
+  <x:si>
+    <x:t>93-58645938-93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(297) 5042126</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Numbat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tasia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaven</x:t>
+  </x:si>
+  <x:si>
+    <x:t>91546708</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72-78884924-07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(645) 1485584</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tortoise, indian star</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Silvan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nealand</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51815122</x:t>
+  </x:si>
+  <x:si>
+    <x:t>61-93615499-36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(876) 6153539</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ibis, puna</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -101,8 +551,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
-  <x:autoFilter ref="A1:H2"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0">
+  <x:autoFilter ref="A1:H51"/>
   <x:tableColumns count="8">
     <x:tableColumn id="1" name="Nombre"/>
     <x:tableColumn id="2" name="Apellido"/>
@@ -405,7 +855,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H2"/>
+  <x:dimension ref="A1:H51"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -435,6 +885,1294 @@
       </x:c>
       <x:c r="H1" s="0" t="s">
         <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
+      <x:c r="A2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="A3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="A4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="A6" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:8">
+      <x:c r="A15" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:8">
+      <x:c r="A16" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:8">
+      <x:c r="A17" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:8">
+      <x:c r="A18" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:8">
+      <x:c r="A19" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:8">
+      <x:c r="A20" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:8">
+      <x:c r="A21" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H21" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:8">
+      <x:c r="A22" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H22" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:8">
+      <x:c r="A23" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H23" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:8">
+      <x:c r="A24" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H24" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:8">
+      <x:c r="A25" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H25" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:8">
+      <x:c r="A26" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H26" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:8">
+      <x:c r="A27" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H27" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:8">
+      <x:c r="A28" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H28" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:8">
+      <x:c r="A29" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H29" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:8">
+      <x:c r="A30" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H30" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:8">
+      <x:c r="A31" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H31" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:8">
+      <x:c r="A32" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="G32" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H32" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:8">
+      <x:c r="A33" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H33" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:8">
+      <x:c r="A34" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="G34" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H34" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:8">
+      <x:c r="A35" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="G35" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H35" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:8">
+      <x:c r="A36" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G36" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H36" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:8">
+      <x:c r="A37" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="G37" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H37" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:8">
+      <x:c r="A38" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="G38" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H38" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:8">
+      <x:c r="A39" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="G39" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H39" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:8">
+      <x:c r="A40" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="G40" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H40" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:8">
+      <x:c r="A41" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="G41" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H41" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:8">
+      <x:c r="A42" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="G42" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H42" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:8">
+      <x:c r="A43" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="G43" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H43" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:8">
+      <x:c r="A44" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="G44" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H44" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:8">
+      <x:c r="A45" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="G45" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H45" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:8">
+      <x:c r="A46" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="G46" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H46" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:8">
+      <x:c r="A47" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="G47" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H47" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:8">
+      <x:c r="A48" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H48" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:8">
+      <x:c r="A49" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="G49" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H49" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:8">
+      <x:c r="A50" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="G50" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H50" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:8">
+      <x:c r="A51" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="G51" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H51" s="0" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>